<commit_message>
change status to bill status
</commit_message>
<xml_diff>
--- a/data/data_customer.xlsx
+++ b/data/data_customer.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="110">
   <si>
     <t>Customer Code</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>0358619390</t>
+  </si>
+  <si>
+    <t>Bill Status</t>
   </si>
 </sst>
 </file>
@@ -733,12 +736,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="152" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -800,7 +804,7 @@
         <v>91</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>